<commit_message>
.xlsx changed, fuzzyST design completed, webster cleared
</commit_message>
<xml_diff>
--- a/trafficcontrolalgorithms.xlsx
+++ b/trafficcontrolalgorithms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Implementations\Mosas Studies\TrafficControlAlgorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED3E2F4-832D-4D54-A18E-F508EE402CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4B0C39-206D-41B1-8B07-F33FD4C3E09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{B799F520-5209-4C24-A23B-39541E2D1861}"/>
   </bookViews>
@@ -50,15 +50,9 @@
     <t>Actuated</t>
   </si>
   <si>
-    <t>Delay Based</t>
-  </si>
-  <si>
     <t>DQN</t>
   </si>
   <si>
-    <t>Max Pressure</t>
-  </si>
-  <si>
     <t>Araç Sayısı</t>
   </si>
   <si>
@@ -92,15 +86,6 @@
     <t>Bekleme süresi odaklı DQN</t>
   </si>
   <si>
-    <t>Fuzzy Signal Time</t>
-  </si>
-  <si>
-    <t>Fuzzy_1</t>
-  </si>
-  <si>
-    <t>Fuzzy_2</t>
-  </si>
-  <si>
     <t>Webster</t>
   </si>
   <si>
@@ -119,16 +104,31 @@
     <t>Verilen süre belirli, Faz sırası önemli</t>
   </si>
   <si>
-    <t>Green Wave</t>
-  </si>
-  <si>
-    <t>Max Band</t>
-  </si>
-  <si>
     <t>SOTL</t>
   </si>
   <si>
     <t>SCATS</t>
+  </si>
+  <si>
+    <t>DelayBased</t>
+  </si>
+  <si>
+    <t>MaxPressure</t>
+  </si>
+  <si>
+    <t>GreenWave</t>
+  </si>
+  <si>
+    <t>MaxBand</t>
+  </si>
+  <si>
+    <t>FuzzyPriority2</t>
+  </si>
+  <si>
+    <t>FuzzyPriority1</t>
+  </si>
+  <si>
+    <t>FuzzySignalTime</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,13 +559,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="3"/>
     </row>
@@ -580,10 +580,10 @@
         <v>715</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -597,15 +597,15 @@
         <v>715</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1">
         <v>7200</v>
@@ -614,15 +614,15 @@
         <v>714</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>7200</v>
@@ -631,15 +631,15 @@
         <v>715</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1">
         <v>7200</v>
@@ -648,15 +648,15 @@
         <v>716</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1">
         <v>7200</v>
@@ -665,48 +665,48 @@
         <v>717</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>7200</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1">
         <v>7200</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1">
+        <v>7200</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="1">
-        <v>7200</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
         <v>7200</v>
@@ -714,7 +714,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1">
         <v>7200</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
         <v>7200</v>
@@ -730,7 +730,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1">
         <v>7200</v>

</xml_diff>

<commit_message>
webster fixed empty phase passing added
</commit_message>
<xml_diff>
--- a/trafficcontrolalgorithms.xlsx
+++ b/trafficcontrolalgorithms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Implementations\Mosas Studies\TrafficControlAlgorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0FBBA0-642E-40C9-91EF-96D3E19655BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2DA128-059F-41F2-B78C-DC54F5647A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B799F520-5209-4C24-A23B-39541E2D1861}"/>
   </bookViews>
@@ -128,10 +128,10 @@
     <t>123.6 saniye</t>
   </si>
   <si>
-    <t>140 saniye</t>
-  </si>
-  <si>
     <t>Webster'sMethod</t>
+  </si>
+  <si>
+    <t>127.6 saniye</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1233,16 +1233,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5">
         <v>7200</v>
       </c>
       <c r="C10" s="5">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>18</v>

</xml_diff>